<commit_message>
- Add CSV version of spreadsheet - Add "How To Use" instructions file - Change name of folder for incremental build scripts
</commit_message>
<xml_diff>
--- a/Pre-Built Datasets/FBI_-_Active_Shooter_Incidents_2000-2018.xlsx
+++ b/Pre-Built Datasets/FBI_-_Active_Shooter_Incidents_2000-2018.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="FBI - Active Shooter Incidents" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -18329,28 +18327,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>